<commit_message>
FIX - Normalização e Desafio 1
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -247,7 +247,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -276,18 +276,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="10">
@@ -408,7 +396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -489,7 +477,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -537,32 +525,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -692,8 +664,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N16" activeCellId="1" sqref="L3:L10 N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -988,11 +960,11 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.51"/>
@@ -1119,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1183,7 +1155,7 @@
         <v>2</v>
       </c>
       <c r="L6" s="30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="L7" s="25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1208,7 +1180,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,14 +1192,14 @@
         <v>3</v>
       </c>
       <c r="L9" s="25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>45</v>
       </c>
       <c r="G10" s="19" t="s">
@@ -1239,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="L10" s="30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,10 +1238,10 @@
       <c r="B12" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="G12" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="34" t="s">
+      <c r="G12" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>48</v>
       </c>
       <c r="I12" s="25" t="n">
@@ -1283,10 +1255,10 @@
       <c r="B13" s="25" t="n">
         <v>14</v>
       </c>
-      <c r="G13" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="36" t="s">
+      <c r="G13" s="33" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="33" t="s">
         <v>49</v>
       </c>
       <c r="I13" s="30" t="n">
@@ -1300,10 +1272,10 @@
       <c r="B14" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="G14" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="H14" s="34" t="s">
+      <c r="G14" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" s="32" t="s">
         <v>50</v>
       </c>
       <c r="I14" s="25" t="n">
@@ -1317,10 +1289,10 @@
       <c r="B15" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="G15" s="35" t="n">
-        <v>4</v>
-      </c>
-      <c r="H15" s="36" t="s">
+      <c r="G15" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="H15" s="33" t="s">
         <v>51</v>
       </c>
       <c r="I15" s="30" t="n">
@@ -1334,10 +1306,10 @@
       <c r="B16" s="30" t="n">
         <v>13</v>
       </c>
-      <c r="G16" s="33" t="n">
+      <c r="G16" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="H16" s="34" t="s">
+      <c r="H16" s="32" t="s">
         <v>52</v>
       </c>
       <c r="I16" s="25" t="n">
@@ -1351,10 +1323,10 @@
       <c r="B17" s="25" t="n">
         <v>15</v>
       </c>
-      <c r="G17" s="35" t="n">
+      <c r="G17" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="H17" s="33" t="s">
         <v>53</v>
       </c>
       <c r="I17" s="30" t="n">
@@ -1368,10 +1340,10 @@
       <c r="B18" s="30" t="n">
         <v>17</v>
       </c>
-      <c r="G18" s="33" t="n">
+      <c r="G18" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="H18" s="34" t="s">
+      <c r="H18" s="32" t="s">
         <v>54</v>
       </c>
       <c r="I18" s="25" t="n">
@@ -1385,10 +1357,10 @@
       <c r="B19" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="G19" s="35" t="n">
+      <c r="G19" s="33" t="n">
         <v>8</v>
       </c>
-      <c r="H19" s="36" t="s">
+      <c r="H19" s="33" t="s">
         <v>55</v>
       </c>
       <c r="I19" s="30" t="n">
@@ -1402,10 +1374,10 @@
       <c r="B20" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="G20" s="33" t="n">
+      <c r="G20" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="H20" s="32" t="s">
         <v>56</v>
       </c>
       <c r="I20" s="25" t="n">
@@ -1419,10 +1391,10 @@
       <c r="B21" s="25" t="n">
         <v>16</v>
       </c>
-      <c r="G21" s="35" t="n">
+      <c r="G21" s="33" t="n">
         <v>10</v>
       </c>
-      <c r="H21" s="36" t="s">
+      <c r="H21" s="33" t="s">
         <v>57</v>
       </c>
       <c r="I21" s="30" t="n">
@@ -1436,10 +1408,10 @@
       <c r="B22" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="33" t="n">
+      <c r="G22" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="32" t="s">
         <v>58</v>
       </c>
       <c r="I22" s="25" t="n">
@@ -1453,10 +1425,10 @@
       <c r="B23" s="25" t="n">
         <v>11</v>
       </c>
-      <c r="G23" s="35" t="n">
+      <c r="G23" s="33" t="n">
         <v>12</v>
       </c>
-      <c r="H23" s="36" t="s">
+      <c r="H23" s="33" t="s">
         <v>59</v>
       </c>
       <c r="I23" s="30" t="n">
@@ -1470,10 +1442,10 @@
       <c r="B24" s="30" t="n">
         <v>18</v>
       </c>
-      <c r="G24" s="33" t="n">
+      <c r="G24" s="32" t="n">
         <v>13</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="32" t="s">
         <v>60</v>
       </c>
       <c r="I24" s="25" t="n">
@@ -1481,10 +1453,10 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="35" t="n">
+      <c r="G25" s="33" t="n">
         <v>14</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="33" t="s">
         <v>61</v>
       </c>
       <c r="I25" s="30" t="n">
@@ -1492,10 +1464,10 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="33" t="n">
+      <c r="G26" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="H26" s="34" t="s">
+      <c r="H26" s="32" t="s">
         <v>62</v>
       </c>
       <c r="I26" s="25" t="n">
@@ -1503,10 +1475,10 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G27" s="35" t="n">
+      <c r="G27" s="33" t="n">
         <v>16</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="33" t="s">
         <v>63</v>
       </c>
       <c r="I27" s="30" t="n">
@@ -1514,21 +1486,21 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G28" s="37" t="n">
+      <c r="G28" s="34" t="n">
         <v>17</v>
       </c>
-      <c r="H28" s="38" t="s">
+      <c r="H28" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="39" t="s">
+      <c r="I28" s="35" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G29" s="40" t="n">
+      <c r="G29" s="36" t="n">
         <v>18</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="33" t="s">
         <v>66</v>
       </c>
       <c r="I29" s="30" t="n">
@@ -1561,10 +1533,10 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+      <selection pane="topLeft" activeCell="K20" activeCellId="1" sqref="L3:L10 K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
@@ -1573,7 +1545,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.68"/>
@@ -1608,7 +1580,7 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="37" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1643,10 +1615,10 @@
       <c r="D3" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="32" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="25" t="n">
@@ -1675,10 +1647,10 @@
       <c r="D4" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="36" t="s">
+      <c r="F4" s="33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="30" t="n">
@@ -1707,10 +1679,10 @@
       <c r="D5" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" s="34" t="s">
+      <c r="F5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="25" t="n">
@@ -1736,13 +1708,13 @@
       <c r="C6" s="27" t="n">
         <v>45</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="35" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" s="36" t="s">
+      <c r="F6" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>51</v>
       </c>
       <c r="H6" s="30" t="n">
@@ -1759,10 +1731,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="33" t="n">
+      <c r="F7" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="32" t="s">
         <v>52</v>
       </c>
       <c r="H7" s="25" t="n">
@@ -1779,10 +1751,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="35" t="n">
+      <c r="F8" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="33" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="30" t="n">
@@ -1795,10 +1767,10 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
-      <c r="F9" s="33" t="n">
+      <c r="F9" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="32" t="s">
         <v>54</v>
       </c>
       <c r="H9" s="25" t="n">
@@ -1806,7 +1778,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1815,10 +1787,10 @@
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="35" t="n">
+      <c r="F10" s="33" t="n">
         <v>8</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="33" t="s">
         <v>55</v>
       </c>
       <c r="H10" s="30" t="n">
@@ -1830,7 +1802,7 @@
       <c r="K10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33" t="n">
+      <c r="A11" s="32" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1839,10 +1811,10 @@
       <c r="C11" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="33" t="n">
+      <c r="F11" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="32" t="s">
         <v>56</v>
       </c>
       <c r="H11" s="25" t="n">
@@ -1856,19 +1828,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="n">
+      <c r="A12" s="33" t="n">
         <v>2</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="44" t="n">
+      <c r="C12" s="40" t="n">
         <v>7.99</v>
       </c>
-      <c r="F12" s="35" t="n">
+      <c r="F12" s="33" t="n">
         <v>10</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="33" t="s">
         <v>57</v>
       </c>
       <c r="H12" s="30" t="n">
@@ -1882,7 +1854,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="n">
+      <c r="A13" s="32" t="n">
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -1891,10 +1863,10 @@
       <c r="C13" s="23" t="n">
         <v>5.99</v>
       </c>
-      <c r="F13" s="33" t="n">
+      <c r="F13" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="32" t="s">
         <v>58</v>
       </c>
       <c r="H13" s="25" t="n">
@@ -1908,10 +1880,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="35" t="n">
+      <c r="F14" s="33" t="n">
         <v>12</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="33" t="s">
         <v>59</v>
       </c>
       <c r="H14" s="30" t="n">
@@ -1925,10 +1897,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="33" t="n">
+      <c r="F15" s="32" t="n">
         <v>13</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="32" t="s">
         <v>60</v>
       </c>
       <c r="H15" s="25" t="n">
@@ -1946,10 +1918,10 @@
         <v>44</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="F16" s="35" t="n">
+      <c r="F16" s="33" t="n">
         <v>14</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="33" t="s">
         <v>61</v>
       </c>
       <c r="H16" s="30" t="n">
@@ -1960,13 +1932,13 @@
       <c r="A17" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="33" t="n">
+      <c r="F17" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="32" t="s">
         <v>62</v>
       </c>
       <c r="H17" s="25" t="n">
@@ -1980,10 +1952,10 @@
       <c r="B18" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="35" t="n">
+      <c r="F18" s="33" t="n">
         <v>16</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="33" t="s">
         <v>63</v>
       </c>
       <c r="H18" s="30" t="n">
@@ -2001,13 +1973,13 @@
       <c r="B19" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="F19" s="37" t="n">
+      <c r="F19" s="34" t="n">
         <v>17</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="35" t="s">
         <v>65</v>
       </c>
       <c r="J19" s="22" t="s">
@@ -2024,10 +1996,10 @@
       <c r="B20" s="25" t="n">
         <v>14</v>
       </c>
-      <c r="F20" s="40" t="n">
+      <c r="F20" s="36" t="n">
         <v>18</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="33" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="30" t="n">
@@ -2051,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2079,7 +2051,7 @@
         <v>2</v>
       </c>
       <c r="K23" s="30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="K24" s="25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2107,7 +2079,7 @@
         <v>3</v>
       </c>
       <c r="K25" s="30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,7 +2093,7 @@
         <v>3</v>
       </c>
       <c r="K26" s="25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,7 +2107,7 @@
         <v>4</v>
       </c>
       <c r="K27" s="30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2197,27 +2169,27 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K27" activeCellId="1" sqref="L3:L10 K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="45" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="45" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="45" width="11.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="45" width="3.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="45" width="10.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="45" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="45" width="9.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="45" width="3.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="45" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="45" width="16.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="45" width="9.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="45" width="3.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="14" style="45" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="46" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="41" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="41" width="11.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="41" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="41" width="3.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="41" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="41" width="21.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="41" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="41" width="3.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="41" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="41" width="16.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="41" width="9.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="41" width="3.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="14" style="41" width="9.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1023" style="42" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2248,7 +2220,7 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="37" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -2283,10 +2255,10 @@
       <c r="D3" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="34" t="s">
+      <c r="F3" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="32" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="25" t="n">
@@ -2315,10 +2287,10 @@
       <c r="D4" s="30" t="n">
         <v>2</v>
       </c>
-      <c r="F4" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="36" t="s">
+      <c r="F4" s="33" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="30" t="n">
@@ -2347,10 +2319,10 @@
       <c r="D5" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="G5" s="34" t="s">
+      <c r="F5" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="25" t="n">
@@ -2376,13 +2348,13 @@
       <c r="C6" s="27" t="n">
         <v>45</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="35" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" s="36" t="s">
+      <c r="F6" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>51</v>
       </c>
       <c r="H6" s="30" t="n">
@@ -2399,10 +2371,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F7" s="33" t="n">
+      <c r="F7" s="32" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="32" t="s">
         <v>52</v>
       </c>
       <c r="H7" s="25" t="n">
@@ -2419,10 +2391,10 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F8" s="35" t="n">
+      <c r="F8" s="33" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="33" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="30" t="n">
@@ -2435,10 +2407,10 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
-      <c r="F9" s="33" t="n">
+      <c r="F9" s="32" t="n">
         <v>7</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="G9" s="32" t="s">
         <v>54</v>
       </c>
       <c r="H9" s="25" t="n">
@@ -2446,7 +2418,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="39" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2455,10 +2427,10 @@
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="35" t="n">
+      <c r="F10" s="33" t="n">
         <v>8</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="33" t="s">
         <v>55</v>
       </c>
       <c r="H10" s="30" t="n">
@@ -2470,7 +2442,7 @@
       <c r="K10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33" t="n">
+      <c r="A11" s="32" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -2479,10 +2451,10 @@
       <c r="C11" s="23" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="33" t="n">
+      <c r="F11" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="32" t="s">
         <v>56</v>
       </c>
       <c r="H11" s="25" t="n">
@@ -2496,19 +2468,19 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="n">
+      <c r="A12" s="33" t="n">
         <v>2</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="44" t="n">
+      <c r="C12" s="40" t="n">
         <v>7.99</v>
       </c>
-      <c r="F12" s="35" t="n">
+      <c r="F12" s="33" t="n">
         <v>10</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="G12" s="33" t="s">
         <v>57</v>
       </c>
       <c r="H12" s="30" t="n">
@@ -2522,7 +2494,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="n">
+      <c r="A13" s="32" t="n">
         <v>3</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -2531,10 +2503,10 @@
       <c r="C13" s="23" t="n">
         <v>5.99</v>
       </c>
-      <c r="F13" s="33" t="n">
+      <c r="F13" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="32" t="s">
         <v>58</v>
       </c>
       <c r="H13" s="25" t="n">
@@ -2548,10 +2520,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="35" t="n">
+      <c r="F14" s="33" t="n">
         <v>12</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="33" t="s">
         <v>59</v>
       </c>
       <c r="H14" s="30" t="n">
@@ -2565,10 +2537,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="33" t="n">
+      <c r="F15" s="32" t="n">
         <v>13</v>
       </c>
-      <c r="G15" s="34" t="s">
+      <c r="G15" s="32" t="s">
         <v>60</v>
       </c>
       <c r="H15" s="25" t="n">
@@ -2586,10 +2558,10 @@
         <v>44</v>
       </c>
       <c r="B16" s="21"/>
-      <c r="F16" s="35" t="n">
+      <c r="F16" s="33" t="n">
         <v>14</v>
       </c>
-      <c r="G16" s="36" t="s">
+      <c r="G16" s="33" t="s">
         <v>61</v>
       </c>
       <c r="H16" s="30" t="n">
@@ -2600,21 +2572,21 @@
       <c r="A17" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="33" t="n">
+      <c r="E17" s="43"/>
+      <c r="F17" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G17" s="32" t="s">
         <v>62</v>
       </c>
       <c r="H17" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="25" t="n">
@@ -2623,11 +2595,11 @@
       <c r="B18" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="35" t="n">
+      <c r="E18" s="43"/>
+      <c r="F18" s="33" t="n">
         <v>16</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="33" t="s">
         <v>63</v>
       </c>
       <c r="H18" s="30" t="n">
@@ -2645,14 +2617,14 @@
       <c r="B19" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="37" t="n">
+      <c r="E19" s="43"/>
+      <c r="F19" s="34" t="n">
         <v>17</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="35" t="s">
         <v>65</v>
       </c>
       <c r="J19" s="22" t="s">
@@ -2669,11 +2641,11 @@
       <c r="B20" s="25" t="n">
         <v>14</v>
       </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="40" t="n">
+      <c r="E20" s="43"/>
+      <c r="F20" s="36" t="n">
         <v>18</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="33" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="30" t="n">
@@ -2693,15 +2665,15 @@
       <c r="B21" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
       <c r="J21" s="29" t="n">
         <v>1</v>
       </c>
       <c r="K21" s="30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2711,10 +2683,10 @@
       <c r="B22" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
       <c r="J22" s="24" t="n">
         <v>1</v>
       </c>
@@ -2729,15 +2701,15 @@
       <c r="B23" s="30" t="n">
         <v>13</v>
       </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
       <c r="J23" s="29" t="n">
         <v>2</v>
       </c>
       <c r="K23" s="30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,15 +2719,15 @@
       <c r="B24" s="25" t="n">
         <v>15</v>
       </c>
-      <c r="E24" s="47"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="47"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="43"/>
       <c r="J24" s="24" t="n">
         <v>2</v>
       </c>
       <c r="K24" s="25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2765,15 +2737,15 @@
       <c r="B25" s="30" t="n">
         <v>17</v>
       </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="47"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="43"/>
       <c r="J25" s="29" t="n">
         <v>3</v>
       </c>
       <c r="K25" s="30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,15 +2755,15 @@
       <c r="B26" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="47"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="43"/>
       <c r="J26" s="24" t="n">
         <v>3</v>
       </c>
       <c r="K26" s="25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2801,15 +2773,15 @@
       <c r="B27" s="30" t="n">
         <v>6</v>
       </c>
-      <c r="E27" s="47"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="47"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="43"/>
       <c r="J27" s="29" t="n">
         <v>4</v>
       </c>
       <c r="K27" s="30" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2819,10 +2791,10 @@
       <c r="B28" s="25" t="n">
         <v>16</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
     </row>

</xml_diff>

<commit_message>
Code corrections and challenge 2
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable.xlsx
+++ b/SpotifyClone-Non-NormalizedTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernanda/Documents/Projects/sd-09-mysql-one-for-all/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C61473-10A0-0646-A7E9-A4F71CA8C252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43403777-5C0B-8642-98DD-4332B8153D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23100" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
   <si>
     <t>usuario_id</t>
   </si>
@@ -205,18 +205,6 @@
     <t>Time Fireworks</t>
   </si>
   <si>
-    <t>Honey</t>
-  </si>
-  <si>
-    <t>So Do I</t>
-  </si>
-  <si>
-    <t>Sweetie</t>
-  </si>
-  <si>
-    <t>Let's Go Wild</t>
-  </si>
-  <si>
     <t>She Knows</t>
   </si>
   <si>
@@ -290,6 +278,12 @@
   </si>
   <si>
     <t>birth_year</t>
+  </si>
+  <si>
+    <t>Honey, So Do I</t>
+  </si>
+  <si>
+    <t>Sweetie, Let's Go Wild</t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1875,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2203,10 +2197,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4107A36C-108B-E245-885F-E32216987BC2}">
-  <dimension ref="B1:G81"/>
+  <dimension ref="B1:G79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64:D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2227,7 +2221,7 @@
     <row r="1" spans="2:7" s="29" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="32"/>
@@ -2236,16 +2230,16 @@
     </row>
     <row r="3" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>73</v>
-      </c>
       <c r="D3" s="33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="33" t="s">
@@ -2331,20 +2325,20 @@
     <row r="8" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
     </row>
     <row r="10" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="33" t="s">
         <v>71</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>75</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="31"/>
@@ -2399,16 +2393,16 @@
     </row>
     <row r="15" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C15" s="32"/>
     </row>
     <row r="16" spans="2:7" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2456,10 +2450,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2472,6 +2466,10 @@
       <c r="D24" s="34">
         <v>1</v>
       </c>
+      <c r="F24" s="29" t="str">
+        <f>_xlfn.CONCAT(B24,", ","'",C24,"'",", ",D24)</f>
+        <v>1, 'Envious', 1</v>
+      </c>
     </row>
     <row r="25" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="34">
@@ -2483,6 +2481,10 @@
       <c r="D25" s="34">
         <v>1</v>
       </c>
+      <c r="F25" s="29" t="str">
+        <f>_xlfn.CONCAT(B25,", ","'",C25,"'",", ",D25)</f>
+        <v>2, 'Exuberant', 1</v>
+      </c>
     </row>
     <row r="26" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="34">
@@ -2494,6 +2496,10 @@
       <c r="D26" s="34">
         <v>2</v>
       </c>
+      <c r="F26" s="29" t="str">
+        <f>_xlfn.CONCAT(B26,", ","'",C26,"'",", ",D26)</f>
+        <v>3, 'Hallowed Steam', 2</v>
+      </c>
     </row>
     <row r="27" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="34">
@@ -2505,6 +2511,10 @@
       <c r="D27" s="34">
         <v>3</v>
       </c>
+      <c r="F27" s="29" t="str">
+        <f>_xlfn.CONCAT(B27,", ","'",C27,"'",", ",D27)</f>
+        <v>4, 'Incandescent', 3</v>
+      </c>
     </row>
     <row r="28" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="34">
@@ -2516,11 +2526,15 @@
       <c r="D28" s="34">
         <v>4</v>
       </c>
+      <c r="F28" s="29" t="str">
+        <f>_xlfn.CONCAT(B28,", ","'",C28,"'",", ",D28)</f>
+        <v>5, 'Temporary Culture', 4</v>
+      </c>
     </row>
     <row r="29" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C30" s="40"/>
       <c r="D30" s="40"/>
@@ -2529,17 +2543,15 @@
     </row>
     <row r="31" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D31" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E31" s="33" t="s">
-        <v>77</v>
-      </c>
+      <c r="E31" s="33"/>
       <c r="F31" s="31"/>
     </row>
     <row r="32" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2552,10 +2564,11 @@
       <c r="D32" s="34">
         <v>1</v>
       </c>
-      <c r="E32" s="34">
-        <v>1</v>
-      </c>
-      <c r="F32" s="28"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="28" t="str">
+        <f>_xlfn.CONCAT("(",B32,", ","'",C32,"'",", ",D32,"),")</f>
+        <v>(1, 'Soul For Us', 1),</v>
+      </c>
     </row>
     <row r="33" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="34">
@@ -2567,10 +2580,11 @@
       <c r="D33" s="34">
         <v>1</v>
       </c>
-      <c r="E33" s="34">
-        <v>1</v>
-      </c>
-      <c r="F33" s="28"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="28" t="str">
+        <f t="shared" ref="F33:F49" si="0">_xlfn.CONCAT("(",B33,", ","'",C33,"'",", ",D33,"),")</f>
+        <v>(2, 'Reflections Of Magic', 1),</v>
+      </c>
     </row>
     <row r="34" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="34">
@@ -2582,10 +2596,11 @@
       <c r="D34" s="34">
         <v>1</v>
       </c>
-      <c r="E34" s="34">
-        <v>1</v>
-      </c>
-      <c r="F34" s="28"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(3, 'Dance With Her Own', 1),</v>
+      </c>
     </row>
     <row r="35" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="34">
@@ -2597,10 +2612,11 @@
       <c r="D35" s="34">
         <v>2</v>
       </c>
-      <c r="E35" s="34">
-        <v>1</v>
-      </c>
-      <c r="F35" s="28"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(4, 'Troubles Of My Inner Fire', 2),</v>
+      </c>
     </row>
     <row r="36" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="34">
@@ -2612,10 +2628,11 @@
       <c r="D36" s="34">
         <v>2</v>
       </c>
-      <c r="E36" s="34">
-        <v>1</v>
-      </c>
-      <c r="F36" s="28"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(5, 'Time Fireworks', 2),</v>
+      </c>
     </row>
     <row r="37" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="34">
@@ -2627,130 +2644,139 @@
       <c r="D37" s="34">
         <v>3</v>
       </c>
-      <c r="E37" s="34">
-        <v>2</v>
-      </c>
-      <c r="F37" s="28"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(6, 'Magic Circus', 3),</v>
+      </c>
     </row>
     <row r="38" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="34">
         <v>7</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="D38" s="34">
         <v>3</v>
       </c>
-      <c r="E38" s="34">
-        <v>2</v>
-      </c>
-      <c r="F38" s="28"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(7, 'Honey, So Do I', 3),</v>
+      </c>
     </row>
     <row r="39" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="34">
         <v>8</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="D39" s="34">
         <v>3</v>
       </c>
-      <c r="E39" s="34">
-        <v>2</v>
-      </c>
-      <c r="F39" s="28"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(8, 'Sweetie, Let's Go Wild', 3),</v>
+      </c>
     </row>
     <row r="40" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="34">
         <v>9</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D40" s="34">
         <v>3</v>
       </c>
-      <c r="E40" s="34">
-        <v>2</v>
-      </c>
-      <c r="F40" s="28"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(9, 'She Knows', 3),</v>
+      </c>
     </row>
     <row r="41" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="34">
         <v>10</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D41" s="34">
-        <v>3</v>
-      </c>
-      <c r="E41" s="34">
-        <v>2</v>
-      </c>
-      <c r="F41" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="E41" s="34"/>
+      <c r="F41" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(10, 'Fantasy For Me', 4),</v>
+      </c>
     </row>
     <row r="42" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="34">
         <v>11</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D42" s="34">
-        <v>3</v>
-      </c>
-      <c r="E42" s="34">
-        <v>2</v>
-      </c>
-      <c r="F42" s="28"/>
+        <v>4</v>
+      </c>
+      <c r="E42" s="34"/>
+      <c r="F42" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(11, 'Celebration Of More', 4),</v>
+      </c>
     </row>
     <row r="43" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="34">
         <v>12</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D43" s="34">
         <v>4</v>
       </c>
-      <c r="E43" s="34">
-        <v>3</v>
-      </c>
-      <c r="F43" s="28"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(12, 'Rock His Everything', 4),</v>
+      </c>
     </row>
     <row r="44" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="34">
         <v>13</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" s="34">
         <v>4</v>
       </c>
-      <c r="E44" s="34">
-        <v>3</v>
-      </c>
-      <c r="F44" s="28"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(13, 'Home Forever', 4),</v>
+      </c>
     </row>
     <row r="45" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="34">
         <v>14</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D45" s="34">
         <v>4</v>
       </c>
-      <c r="E45" s="34">
-        <v>3</v>
-      </c>
-      <c r="F45" s="28"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(14, 'Diamond Power', 4),</v>
+      </c>
     </row>
     <row r="46" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="34">
@@ -2762,99 +2788,97 @@
       <c r="D46" s="34">
         <v>4</v>
       </c>
-      <c r="E46" s="34">
-        <v>3</v>
-      </c>
-      <c r="F46" s="28"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(15, 'Honey, Let's Be Silly', 4),</v>
+      </c>
     </row>
     <row r="47" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="34">
         <v>16</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D47" s="34">
-        <v>4</v>
-      </c>
-      <c r="E47" s="34">
-        <v>3</v>
-      </c>
-      <c r="F47" s="28"/>
+        <v>5</v>
+      </c>
+      <c r="E47" s="34"/>
+      <c r="F47" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(16, 'Thang Of Thunder', 5),</v>
+      </c>
     </row>
     <row r="48" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="34">
         <v>17</v>
       </c>
       <c r="C48" s="36" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D48" s="34">
-        <v>4</v>
-      </c>
-      <c r="E48" s="34">
-        <v>3</v>
-      </c>
-      <c r="F48" s="28"/>
+        <v>5</v>
+      </c>
+      <c r="E48" s="34"/>
+      <c r="F48" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(17, 'Words Of Her Life', 5),</v>
+      </c>
     </row>
     <row r="49" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="34">
         <v>18</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D49" s="34">
         <v>5</v>
       </c>
-      <c r="E49" s="34">
-        <v>4</v>
-      </c>
-      <c r="F49" s="28"/>
-    </row>
-    <row r="50" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="34">
-        <v>19</v>
-      </c>
-      <c r="C50" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D50" s="34">
-        <v>5</v>
-      </c>
-      <c r="E50" s="34">
-        <v>4</v>
-      </c>
-      <c r="F50" s="28"/>
-    </row>
+      <c r="E49" s="34"/>
+      <c r="F49" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>(18, 'Without My Streets', 5),</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="34">
-        <v>20</v>
-      </c>
-      <c r="C51" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="D51" s="34">
-        <v>5</v>
-      </c>
-      <c r="E51" s="34">
-        <v>4</v>
-      </c>
-      <c r="F51" s="28"/>
-    </row>
-    <row r="52" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="B51" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C51" s="32"/>
+    </row>
+    <row r="52" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>73</v>
+      </c>
+    </row>
     <row r="53" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C53" s="32"/>
+      <c r="B53" s="42">
+        <v>1</v>
+      </c>
+      <c r="C53" s="42">
+        <v>1</v>
+      </c>
+      <c r="D53" s="29" t="str">
+        <f>_xlfn.CONCAT("(",B53,", ",C53,"),")</f>
+        <v>(1, 1),</v>
+      </c>
     </row>
     <row r="54" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C54" s="38" t="s">
-        <v>77</v>
+      <c r="B54" s="42">
+        <v>1</v>
+      </c>
+      <c r="C54" s="42">
+        <v>3</v>
+      </c>
+      <c r="D54" s="29" t="str">
+        <f t="shared" ref="D54:D60" si="1">_xlfn.CONCAT("(",B54,", ",C54,"),")</f>
+        <v>(1, 3),</v>
       </c>
     </row>
     <row r="55" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2862,200 +2886,264 @@
         <v>1</v>
       </c>
       <c r="C55" s="42">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D55" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>(1, 4),</v>
       </c>
     </row>
     <row r="56" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="42">
+        <v>2</v>
+      </c>
+      <c r="C56" s="42">
         <v>1</v>
       </c>
-      <c r="C56" s="42">
-        <v>3</v>
+      <c r="D56" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>(2, 1),</v>
       </c>
     </row>
     <row r="57" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" s="42">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="D57" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>(2, 3),</v>
       </c>
     </row>
     <row r="58" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" s="42">
         <v>1</v>
       </c>
+      <c r="D58" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 1),</v>
+      </c>
     </row>
     <row r="59" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="42">
+        <v>3</v>
+      </c>
+      <c r="C59" s="42">
         <v>2</v>
       </c>
-      <c r="C59" s="42">
-        <v>3</v>
+      <c r="D59" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>(3, 2),</v>
       </c>
     </row>
     <row r="60" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="42">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C60" s="42">
+        <v>4</v>
+      </c>
+      <c r="D60" s="29" t="str">
+        <f t="shared" si="1"/>
+        <v>(4, 4),</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" s="41"/>
+      <c r="D62" s="43"/>
+    </row>
+    <row r="63" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="42">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="42">
-        <v>3</v>
-      </c>
-      <c r="C61" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="42">
-        <v>4</v>
-      </c>
-      <c r="C62" s="42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="2:6" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="43"/>
-    </row>
-    <row r="65" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" s="38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="42">
+        <v>1</v>
+      </c>
+      <c r="D64" s="29" t="str">
+        <f>_xlfn.CONCAT("(",B64,", ",C64,"),")</f>
+        <v>(1, 1),</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="42">
+        <v>1</v>
+      </c>
+      <c r="C65" s="42">
+        <v>6</v>
+      </c>
+      <c r="D65" s="29" t="str">
+        <f t="shared" ref="D65:D77" si="2">_xlfn.CONCAT("(",B65,", ",C65,"),")</f>
+        <v>(1, 6),</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="42">
         <v>1</v>
       </c>
       <c r="C66" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="D66" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(1, 14),</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="42">
         <v>1</v>
       </c>
       <c r="C67" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D67" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(1, 16),</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C68" s="42">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="D68" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(2, 13),</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C69" s="42">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="D69" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(2, 17),</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="42">
         <v>2</v>
       </c>
       <c r="C70" s="42">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D70" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(2, 2),</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="42">
         <v>2</v>
       </c>
       <c r="C71" s="42">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="D71" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(2, 15),</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B72" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C72" s="42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="D72" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(3, 4),</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C73" s="42">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="D73" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(3, 16),</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B74" s="42">
         <v>3</v>
       </c>
       <c r="C74" s="42">
+        <v>6</v>
+      </c>
+      <c r="D74" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(3, 6),</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="42">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="42">
+      <c r="C75" s="42">
         <v>3</v>
       </c>
-      <c r="C75" s="42">
+      <c r="D75" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(4, 3),</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="42">
+        <v>4</v>
+      </c>
+      <c r="C76" s="42">
         <v>18</v>
       </c>
-    </row>
-    <row r="76" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="42">
-        <v>3</v>
-      </c>
-      <c r="C76" s="42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D76" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(4, 18),</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B77" s="42">
         <v>4</v>
       </c>
       <c r="C77" s="42">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="42">
-        <v>4</v>
-      </c>
-      <c r="C78" s="42">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="42">
-        <v>4</v>
-      </c>
-      <c r="C79" s="42">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>11</v>
+      </c>
+      <c r="D77" s="29" t="str">
+        <f t="shared" si="2"/>
+        <v>(4, 11),</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="2:4" s="29" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B51:C51"/>
     <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B62:C62"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B9:D9"/>

</xml_diff>